<commit_message>
Cambio di segno alle derivate di controllo del latero direzionale
</commit_message>
<xml_diff>
--- a/ANALYSIS RESULTS/confronto_con_software.xlsx
+++ b/ANALYSIS RESULTS/confronto_con_software.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="216">
   <si>
     <t>Stability_derivative</t>
   </si>
@@ -101,6 +101,330 @@
   </si>
   <si>
     <t>CZ</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>delta_e</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>delta_r</t>
+  </si>
+  <si>
+    <t>delta_a</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>delta_e</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>delta_r</t>
+  </si>
+  <si>
+    <t>delta_a</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>delta_e</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>delta_r</t>
+  </si>
+  <si>
+    <t>delta_a</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>delta_e</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Stability_derivative</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>XFLR5</t>
+  </si>
+  <si>
+    <t>Open VSP</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>delta_r</t>
+  </si>
+  <si>
+    <t>delta_a</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
   <si>
     <t>Stability_derivative</t>
@@ -723,38 +1047,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.42578125" customWidth="true"/>
-    <col min="4" max="4" width="9.85546875" customWidth="true"/>
-    <col min="5" max="5" width="5.140625" customWidth="true"/>
-    <col min="6" max="6" width="7.42578125" customWidth="true"/>
-    <col min="7" max="7" width="7.7109375" customWidth="true"/>
-    <col min="8" max="8" width="3.85546875" customWidth="true"/>
-    <col min="9" max="9" width="3.85546875" customWidth="true"/>
+    <col min="3" max="3" width="16.6015625" customWidth="true"/>
+    <col min="4" max="4" width="8.93359375" customWidth="true"/>
+    <col min="5" max="5" width="4.82421875" customWidth="true"/>
+    <col min="6" max="6" width="6.93359375" customWidth="true"/>
+    <col min="7" max="7" width="7.26953125" customWidth="true"/>
+    <col min="8" max="8" width="3.82421875" customWidth="true"/>
+    <col min="9" max="9" width="3.82421875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="2" x14ac:dyDescent="0.25">
       <c r="C2" s="0" t="s">
-        <v>81</v>
+        <v>189</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>90</v>
+        <v>198</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
       <c r="C3" s="0" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="E3" s="0">
         <v>-100</v>
@@ -768,10 +1092,10 @@
     </row>
     <row r="4" x14ac:dyDescent="0.25">
       <c r="C4" s="0" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>86</v>
+        <v>194</v>
       </c>
       <c r="E4" s="0">
         <v>-100</v>
@@ -785,10 +1109,10 @@
     </row>
     <row r="5" x14ac:dyDescent="0.25">
       <c r="C5" s="0" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="E5" s="0">
         <v>-100</v>
@@ -802,10 +1126,10 @@
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="C6" s="0" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>88</v>
+        <v>196</v>
       </c>
       <c r="E6" s="0">
         <v>-100</v>
@@ -819,42 +1143,42 @@
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="C9" s="0" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>96</v>
+        <v>204</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>106</v>
+        <v>214</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>107</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
       <c r="C10" s="0" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>97</v>
+        <v>205</v>
       </c>
       <c r="E10" s="1">
         <v>-5.7230857142857037</v>
       </c>
       <c r="F10" s="1">
-        <v>-270.88485714285713</v>
+        <v>70.884857142857157</v>
       </c>
       <c r="G10" s="1">
-        <v>-138.5251320754717</v>
+        <v>-61.474867924528297</v>
       </c>
       <c r="H10" s="1">
         <v>-53.094984025559114</v>
@@ -865,19 +1189,19 @@
     </row>
     <row r="11" x14ac:dyDescent="0.25">
       <c r="C11" s="0" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E11" s="1">
         <v>7.1328571428571506</v>
       </c>
       <c r="F11" s="1">
-        <v>-217.1208224543081</v>
+        <v>17.120822454308097</v>
       </c>
       <c r="G11" s="1">
-        <v>-90.027682539682544</v>
+        <v>-109.97231746031748</v>
       </c>
       <c r="H11" s="1">
         <v>-54.54715170278638</v>
@@ -888,19 +1212,19 @@
     </row>
     <row r="12" x14ac:dyDescent="0.25">
       <c r="C12" s="0" t="s">
-        <v>94</v>
+        <v>202</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="E12" s="1">
         <v>323.66123076923083</v>
       </c>
       <c r="F12" s="1">
-        <v>450.18367139959435</v>
+        <v>-250.18367139959437</v>
       </c>
       <c r="G12" s="1">
-        <v>-183.81306122448979</v>
+        <v>-16.1869387755102</v>
       </c>
       <c r="H12" s="1">
         <v>2.4525441696113157</v>
@@ -911,19 +1235,19 @@
     </row>
     <row r="13" x14ac:dyDescent="0.25">
       <c r="C13" s="0" t="s">
-        <v>94</v>
+        <v>202</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="E13" s="1">
         <v>-20.410462427745664</v>
       </c>
       <c r="F13" s="1">
-        <v>-235.93744094488193</v>
+        <v>35.937440944881885</v>
       </c>
       <c r="G13" s="1">
-        <v>-197.011968503937</v>
+        <v>-2.9880314960629928</v>
       </c>
       <c r="H13" s="1">
         <v>6.5958455882352842</v>
@@ -934,19 +1258,19 @@
     </row>
     <row r="14" x14ac:dyDescent="0.25">
       <c r="C14" s="0" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>101</v>
+        <v>209</v>
       </c>
       <c r="E14" s="1">
         <v>3.5462808842652813</v>
       </c>
       <c r="F14" s="1">
-        <v>-283.03658333333328</v>
+        <v>83.03658333333334</v>
       </c>
       <c r="G14" s="1">
-        <v>-142.18380341880342</v>
+        <v>-57.816196581196586</v>
       </c>
       <c r="H14" s="1">
         <v>-92.759813905930471</v>
@@ -957,19 +1281,19 @@
     </row>
     <row r="15" x14ac:dyDescent="0.25">
       <c r="C15" s="0" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>102</v>
+        <v>210</v>
       </c>
       <c r="E15" s="1">
         <v>-0.34156445556946335</v>
       </c>
       <c r="F15" s="1">
-        <v>-220.68346153846156</v>
+        <v>20.683461538461533</v>
       </c>
       <c r="G15" s="1">
-        <v>-92.578187969924812</v>
+        <v>-107.42181203007519</v>
       </c>
       <c r="H15" s="1">
         <v>-91.137794743429296</v>

</xml_diff>